<commit_message>
fixes for api & web demo tests
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10412"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C29478-6610-4643-9B69-C60E11B64524}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="32200" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSMArena" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Execute</t>
   </si>
@@ -38,57 +39,12 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>Z2</t>
-  </si>
-  <si>
-    <t>5MP</t>
-  </si>
-  <si>
-    <t>13MP</t>
-  </si>
-  <si>
-    <t>12MP</t>
-  </si>
-  <si>
     <t>brand</t>
   </si>
   <si>
-    <t>Galaxy S7 active</t>
-  </si>
-  <si>
-    <t>Galaxy On7 Pro</t>
-  </si>
-  <si>
     <t>model</t>
   </si>
   <si>
-    <t>4.0"</t>
-  </si>
-  <si>
-    <t>5.5"</t>
-  </si>
-  <si>
-    <t>5.1"</t>
-  </si>
-  <si>
-    <t>1GB RAM</t>
-  </si>
-  <si>
-    <t>2GB RAM</t>
-  </si>
-  <si>
-    <t>4GB RAM</t>
-  </si>
-  <si>
-    <t>1500mAh</t>
-  </si>
-  <si>
-    <t>3000mAh</t>
-  </si>
-  <si>
-    <t>4000mAh</t>
-  </si>
-  <si>
     <t>GSMA0001</t>
   </si>
   <si>
@@ -135,13 +91,55 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Galaxy S10+</t>
+  </si>
+  <si>
+    <t>6.4"</t>
+  </si>
+  <si>
+    <t>16MP</t>
+  </si>
+  <si>
+    <t>12GB RAM</t>
+  </si>
+  <si>
+    <t>4100mAh</t>
+  </si>
+  <si>
+    <t>Galaxy S10</t>
+  </si>
+  <si>
+    <t>6.1"</t>
+  </si>
+  <si>
+    <t>8GB RAM</t>
+  </si>
+  <si>
+    <t>3400mAh</t>
+  </si>
+  <si>
+    <t>Galaxy View2</t>
+  </si>
+  <si>
+    <t>17.3"</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>3GB RAM</t>
+  </si>
+  <si>
+    <t>12000mAh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +155,12 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,9 +194,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -208,9 +213,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -248,7 +253,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -354,7 +359,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,22 +532,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,10 +555,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -562,90 +567,90 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
+      <c r="D2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -656,21 +661,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,61 +683,61 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="E4">
         <v>100</v>

</xml_diff>

<commit_message>
updated description for retry regression tests
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C29478-6610-4643-9B69-C60E11B64524}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FB041-8EF0-4B16-8DAC-D7D4B8A02426}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="32200" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSMArena" sheetId="1" r:id="rId1"/>
     <sheet name="Calculator" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Execute</t>
   </si>
@@ -133,13 +134,25 @@
   </si>
   <si>
     <t>12000mAh</t>
+  </si>
+  <si>
+    <t>arg1</t>
+  </si>
+  <si>
+    <t>arg2</t>
+  </si>
+  <si>
+    <t>arg3</t>
+  </si>
+  <si>
+    <t>arg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -195,6 +208,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,19 +555,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -600,7 +620,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -627,7 +647,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -668,14 +688,14 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,7 +712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -709,7 +729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -726,7 +746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -746,4 +766,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159BBBDB-2C19-4029-8CF8-DF830F70E1A1}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2:B4" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated XlsDataproviderRetryTest logic to cover cases better
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041FB041-8EF0-4B16-8DAC-D7D4B8A02426}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1309E46-3000-43DF-A3CA-2B5D28B07283}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="68">
   <si>
     <t>Execute</t>
   </si>
@@ -145,14 +145,89 @@
     <t>arg3</t>
   </si>
   <si>
-    <t>arg</t>
+    <t>TestTitle</t>
+  </si>
+  <si>
+    <t>Args</t>
+  </si>
+  <si>
+    <t>tuid1</t>
+  </si>
+  <si>
+    <t>title1</t>
+  </si>
+  <si>
+    <t>tuid2</t>
+  </si>
+  <si>
+    <t>title2</t>
+  </si>
+  <si>
+    <t>tuid3</t>
+  </si>
+  <si>
+    <t>title3</t>
+  </si>
+  <si>
+    <t>tuid4</t>
+  </si>
+  <si>
+    <t>title4</t>
+  </si>
+  <si>
+    <t>arg4</t>
+  </si>
+  <si>
+    <t>tuid5</t>
+  </si>
+  <si>
+    <t>title5</t>
+  </si>
+  <si>
+    <t>arg5</t>
+  </si>
+  <si>
+    <t>tuid6</t>
+  </si>
+  <si>
+    <t>title6</t>
+  </si>
+  <si>
+    <t>arg6</t>
+  </si>
+  <si>
+    <t>tuid7</t>
+  </si>
+  <si>
+    <t>title7</t>
+  </si>
+  <si>
+    <t>arg7</t>
+  </si>
+  <si>
+    <t>tuid8</t>
+  </si>
+  <si>
+    <t>title8</t>
+  </si>
+  <si>
+    <t>arg8</t>
+  </si>
+  <si>
+    <t>tuid9</t>
+  </si>
+  <si>
+    <t>title9</t>
+  </si>
+  <si>
+    <t>arg9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,13 +250,45 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="31"/>
+        <bgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="50"/>
+        <bgColor indexed="55"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -193,10 +300,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,18 +316,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{54382045-ACAB-4016-8E48-6E3B48DC3618}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -770,67 +890,223 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159BBBDB-2C19-4029-8CF8-DF830F70E1A1}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D1" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="D1">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="B2:B4" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed ui tests verifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1309E46-3000-43DF-A3CA-2B5D28B07283}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3F057E-6092-4A9C-BBE8-1F3B545D07FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GSMArena" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>6.1"</t>
   </si>
   <si>
-    <t>8GB RAM</t>
-  </si>
-  <si>
     <t>3400mAh</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>arg9</t>
+  </si>
+  <si>
+    <t>8/12GB RAM</t>
   </si>
 </sst>
 </file>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -685,6 +685,7 @@
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -760,10 +761,10 @@
         <v>27</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -778,19 +779,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -892,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159BBBDB-2C19-4029-8CF8-DF830F70E1A1}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -912,10 +913,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -923,13 +924,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -937,13 +938,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -951,13 +952,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -965,13 +966,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -979,13 +980,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -993,13 +994,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1007,13 +1008,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1021,13 +1022,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1035,13 +1036,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>

<commit_message>
#59: fixed data provider RAM values for validation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3F057E-6092-4A9C-BBE8-1F3B545D07FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A6C4C9-8BC0-4808-BEC7-FAD91032B517}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>16MP</t>
   </si>
   <si>
-    <t>12GB RAM</t>
-  </si>
-  <si>
     <t>4100mAh</t>
   </si>
   <si>
@@ -221,6 +218,9 @@
   </si>
   <si>
     <t>8/12GB RAM</t>
+  </si>
+  <si>
+    <t>8GB RAM</t>
   </si>
 </sst>
 </file>
@@ -734,10 +734,10 @@
         <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -752,10 +752,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>27</v>
@@ -764,7 +764,7 @@
         <v>67</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -779,19 +779,19 @@
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -913,10 +913,10 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -924,13 +924,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -938,13 +938,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="D3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -952,13 +952,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -966,13 +966,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -980,13 +980,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -994,13 +994,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1008,13 +1008,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="D8" s="7" t="s">
         <v>59</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1022,13 +1022,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1036,13 +1036,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4">

</xml_diff>